<commit_message>
Commit: progress bar update
</commit_message>
<xml_diff>
--- a/Solutions(1).xlsx
+++ b/Solutions(1).xlsx
@@ -626,7 +626,7 @@
     <t>Colin Farrell</t>
   </si>
   <si>
-    <t>Assessing When it is Appropriate to do Data Mining and/or Machine Learning</t>
+    <t>Deep Learning for protein subcellular localisation prediction</t>
   </si>
   <si>
     <t>None</t>
@@ -635,43 +635,43 @@
     <t>Enrico Caruso</t>
   </si>
   <si>
+    <t>Narrative Emotion</t>
+  </si>
+  <si>
+    <t>Charlie Brown</t>
+  </si>
+  <si>
+    <t>Deep Colourisation</t>
+  </si>
+  <si>
+    <t>Austin Powers</t>
+  </si>
+  <si>
+    <t>Data Analytics for AHA Case History Forms</t>
+  </si>
+  <si>
+    <t>Alan Sugar</t>
+  </si>
+  <si>
     <t xml:space="preserve">Forecasting Electricity Load for Commercial Buildings </t>
   </si>
   <si>
-    <t>Charlie Brown</t>
-  </si>
-  <si>
-    <t>Graph Indexing: Case Study on Textile Structure</t>
-  </si>
-  <si>
-    <t>Austin Powers</t>
-  </si>
-  <si>
-    <t>Give Your Skills: Volunteer Platform for Project Management</t>
-  </si>
-  <si>
-    <t>Alan Sugar</t>
-  </si>
-  <si>
-    <t>Deep Learning for protein subcellular localisation prediction</t>
-  </si>
-  <si>
     <t>Adam Sandler</t>
   </si>
   <si>
-    <t>Predicting Protein Contact Maps post-Google</t>
+    <t>Standalone Software Metrics Tool</t>
   </si>
   <si>
     <t>Basil Fawlty</t>
   </si>
   <si>
-    <t>Deep Colourisation</t>
+    <t xml:space="preserve">Investigating Wavelet-Based Symbolic Representations for Time Series Classification </t>
   </si>
   <si>
     <t>Ann Coulter</t>
   </si>
   <si>
-    <t>Identifying systematic bias in Bayesian statistical modelling</t>
+    <t>Simulation of Hadoop Task Scheduling Algorithms in Distributed Computing Environments</t>
   </si>
 </sst>
 </file>

</xml_diff>